<commit_message>
updated RMD legacy forms
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-3CE-update.xlsx
+++ b/form_reporting_templates/Form-3CE-update.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAEC914-2CA4-416E-A8D2-4499DCB710FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D916957-CC9F-4552-A38B-2D6382EB7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="JaUivJj1XpzVIsMUuIWG4pvRwNkhjECqAfRNMoS0pEzY8qCMrWJoKRkwK5J/dPq5W+eH0fv+0nU0ZPhh5rEo8w==" workbookSaltValue="WSrsrEWzygKOJ9WtcOLB6A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -164,8 +164,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -644,10 +644,10 @@
   <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -832,6 +832,10 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -891,10 +895,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1222,7 +1222,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,24 +1237,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="74"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1304,15 +1304,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="68"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="68"/>
+      <c r="G8" s="69"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
       <c r="C12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="83"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1366,7 +1366,7 @@
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="83"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1479,10 +1479,10 @@
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="68"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1610,11 +1610,11 @@
     </row>
     <row r="36" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="68"/>
       <c r="H36" s="11"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1695,338 +1695,338 @@
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="70"/>
-      <c r="AK2" s="70"/>
-      <c r="AL2" s="70"/>
-      <c r="AM2" s="70"/>
-      <c r="AN2" s="70"/>
-      <c r="AO2" s="70"/>
-      <c r="AP2" s="70"/>
-      <c r="AQ2" s="70"/>
-      <c r="AR2" s="70"/>
-      <c r="AS2" s="70"/>
-      <c r="AT2" s="70"/>
-      <c r="AU2" s="70"/>
-      <c r="AV2" s="70"/>
-      <c r="AW2" s="70"/>
-      <c r="AX2" s="70"/>
-      <c r="AY2" s="70"/>
-      <c r="AZ2" s="70"/>
-      <c r="BA2" s="70"/>
-      <c r="BB2" s="70"/>
-      <c r="BC2" s="70"/>
-      <c r="BD2" s="70"/>
-      <c r="BE2" s="70"/>
-      <c r="BF2" s="70"/>
-      <c r="BG2" s="70"/>
-      <c r="BH2" s="70"/>
-      <c r="BI2" s="70"/>
-      <c r="BJ2" s="70"/>
-      <c r="BK2" s="70"/>
-      <c r="BL2" s="70"/>
-      <c r="BM2" s="70"/>
-      <c r="BN2" s="70"/>
-      <c r="BO2" s="70"/>
-      <c r="BP2" s="70"/>
-      <c r="BQ2" s="70"/>
-      <c r="BR2" s="70"/>
-      <c r="BS2" s="70"/>
-      <c r="BT2" s="70"/>
-      <c r="BU2" s="70"/>
-      <c r="BV2" s="70"/>
-      <c r="BW2" s="70"/>
-      <c r="BX2" s="70"/>
-      <c r="BY2" s="70"/>
-      <c r="BZ2" s="70"/>
-      <c r="CA2" s="70"/>
-      <c r="CB2" s="70"/>
-      <c r="CC2" s="70"/>
-      <c r="CD2" s="70"/>
-      <c r="CE2" s="70"/>
-      <c r="CF2" s="70"/>
-      <c r="CG2" s="70"/>
-      <c r="CH2" s="70"/>
-      <c r="CI2" s="70"/>
-      <c r="CJ2" s="70"/>
-      <c r="CK2" s="70"/>
-      <c r="CL2" s="70"/>
-      <c r="CM2" s="70"/>
-      <c r="CN2" s="70"/>
-      <c r="CO2" s="70"/>
-      <c r="CP2" s="70"/>
-      <c r="CQ2" s="70"/>
-      <c r="CR2" s="70"/>
-      <c r="CS2" s="70"/>
-      <c r="CT2" s="70"/>
-      <c r="CU2" s="70"/>
-      <c r="CV2" s="70"/>
-      <c r="CW2" s="70"/>
-      <c r="CX2" s="70"/>
-      <c r="CY2" s="70"/>
-      <c r="CZ2" s="70"/>
-      <c r="DA2" s="70"/>
-      <c r="DB2" s="70"/>
-      <c r="DC2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="71"/>
+      <c r="AK2" s="71"/>
+      <c r="AL2" s="71"/>
+      <c r="AM2" s="71"/>
+      <c r="AN2" s="71"/>
+      <c r="AO2" s="71"/>
+      <c r="AP2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+      <c r="AT2" s="71"/>
+      <c r="AU2" s="71"/>
+      <c r="AV2" s="71"/>
+      <c r="AW2" s="71"/>
+      <c r="AX2" s="71"/>
+      <c r="AY2" s="71"/>
+      <c r="AZ2" s="71"/>
+      <c r="BA2" s="71"/>
+      <c r="BB2" s="71"/>
+      <c r="BC2" s="71"/>
+      <c r="BD2" s="71"/>
+      <c r="BE2" s="71"/>
+      <c r="BF2" s="71"/>
+      <c r="BG2" s="71"/>
+      <c r="BH2" s="71"/>
+      <c r="BI2" s="71"/>
+      <c r="BJ2" s="71"/>
+      <c r="BK2" s="71"/>
+      <c r="BL2" s="71"/>
+      <c r="BM2" s="71"/>
+      <c r="BN2" s="71"/>
+      <c r="BO2" s="71"/>
+      <c r="BP2" s="71"/>
+      <c r="BQ2" s="71"/>
+      <c r="BR2" s="71"/>
+      <c r="BS2" s="71"/>
+      <c r="BT2" s="71"/>
+      <c r="BU2" s="71"/>
+      <c r="BV2" s="71"/>
+      <c r="BW2" s="71"/>
+      <c r="BX2" s="71"/>
+      <c r="BY2" s="71"/>
+      <c r="BZ2" s="71"/>
+      <c r="CA2" s="71"/>
+      <c r="CB2" s="71"/>
+      <c r="CC2" s="71"/>
+      <c r="CD2" s="71"/>
+      <c r="CE2" s="71"/>
+      <c r="CF2" s="71"/>
+      <c r="CG2" s="71"/>
+      <c r="CH2" s="71"/>
+      <c r="CI2" s="71"/>
+      <c r="CJ2" s="71"/>
+      <c r="CK2" s="71"/>
+      <c r="CL2" s="71"/>
+      <c r="CM2" s="71"/>
+      <c r="CN2" s="71"/>
+      <c r="CO2" s="71"/>
+      <c r="CP2" s="71"/>
+      <c r="CQ2" s="71"/>
+      <c r="CR2" s="71"/>
+      <c r="CS2" s="71"/>
+      <c r="CT2" s="71"/>
+      <c r="CU2" s="71"/>
+      <c r="CV2" s="71"/>
+      <c r="CW2" s="71"/>
+      <c r="CX2" s="71"/>
+      <c r="CY2" s="71"/>
+      <c r="CZ2" s="71"/>
+      <c r="DA2" s="71"/>
+      <c r="DB2" s="71"/>
+      <c r="DC2" s="72"/>
     </row>
     <row r="3" spans="2:107" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="73"/>
-      <c r="AC3" s="73"/>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="73"/>
-      <c r="AI3" s="73"/>
-      <c r="AJ3" s="73"/>
-      <c r="AK3" s="73"/>
-      <c r="AL3" s="73"/>
-      <c r="AM3" s="73"/>
-      <c r="AN3" s="73"/>
-      <c r="AO3" s="73"/>
-      <c r="AP3" s="73"/>
-      <c r="AQ3" s="73"/>
-      <c r="AR3" s="73"/>
-      <c r="AS3" s="73"/>
-      <c r="AT3" s="73"/>
-      <c r="AU3" s="73"/>
-      <c r="AV3" s="73"/>
-      <c r="AW3" s="73"/>
-      <c r="AX3" s="73"/>
-      <c r="AY3" s="73"/>
-      <c r="AZ3" s="73"/>
-      <c r="BA3" s="73"/>
-      <c r="BB3" s="73"/>
-      <c r="BC3" s="73"/>
-      <c r="BD3" s="73"/>
-      <c r="BE3" s="73"/>
-      <c r="BF3" s="73"/>
-      <c r="BG3" s="73"/>
-      <c r="BH3" s="73"/>
-      <c r="BI3" s="73"/>
-      <c r="BJ3" s="73"/>
-      <c r="BK3" s="73"/>
-      <c r="BL3" s="73"/>
-      <c r="BM3" s="73"/>
-      <c r="BN3" s="73"/>
-      <c r="BO3" s="73"/>
-      <c r="BP3" s="73"/>
-      <c r="BQ3" s="73"/>
-      <c r="BR3" s="73"/>
-      <c r="BS3" s="73"/>
-      <c r="BT3" s="73"/>
-      <c r="BU3" s="73"/>
-      <c r="BV3" s="73"/>
-      <c r="BW3" s="73"/>
-      <c r="BX3" s="73"/>
-      <c r="BY3" s="73"/>
-      <c r="BZ3" s="73"/>
-      <c r="CA3" s="73"/>
-      <c r="CB3" s="73"/>
-      <c r="CC3" s="73"/>
-      <c r="CD3" s="73"/>
-      <c r="CE3" s="73"/>
-      <c r="CF3" s="73"/>
-      <c r="CG3" s="73"/>
-      <c r="CH3" s="73"/>
-      <c r="CI3" s="73"/>
-      <c r="CJ3" s="73"/>
-      <c r="CK3" s="73"/>
-      <c r="CL3" s="73"/>
-      <c r="CM3" s="73"/>
-      <c r="CN3" s="73"/>
-      <c r="CO3" s="73"/>
-      <c r="CP3" s="73"/>
-      <c r="CQ3" s="73"/>
-      <c r="CR3" s="73"/>
-      <c r="CS3" s="73"/>
-      <c r="CT3" s="73"/>
-      <c r="CU3" s="73"/>
-      <c r="CV3" s="73"/>
-      <c r="CW3" s="73"/>
-      <c r="CX3" s="73"/>
-      <c r="CY3" s="73"/>
-      <c r="CZ3" s="73"/>
-      <c r="DA3" s="73"/>
-      <c r="DB3" s="73"/>
-      <c r="DC3" s="74"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
+      <c r="AC3" s="74"/>
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="74"/>
+      <c r="AF3" s="74"/>
+      <c r="AG3" s="74"/>
+      <c r="AH3" s="74"/>
+      <c r="AI3" s="74"/>
+      <c r="AJ3" s="74"/>
+      <c r="AK3" s="74"/>
+      <c r="AL3" s="74"/>
+      <c r="AM3" s="74"/>
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="74"/>
+      <c r="AP3" s="74"/>
+      <c r="AQ3" s="74"/>
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="74"/>
+      <c r="AT3" s="74"/>
+      <c r="AU3" s="74"/>
+      <c r="AV3" s="74"/>
+      <c r="AW3" s="74"/>
+      <c r="AX3" s="74"/>
+      <c r="AY3" s="74"/>
+      <c r="AZ3" s="74"/>
+      <c r="BA3" s="74"/>
+      <c r="BB3" s="74"/>
+      <c r="BC3" s="74"/>
+      <c r="BD3" s="74"/>
+      <c r="BE3" s="74"/>
+      <c r="BF3" s="74"/>
+      <c r="BG3" s="74"/>
+      <c r="BH3" s="74"/>
+      <c r="BI3" s="74"/>
+      <c r="BJ3" s="74"/>
+      <c r="BK3" s="74"/>
+      <c r="BL3" s="74"/>
+      <c r="BM3" s="74"/>
+      <c r="BN3" s="74"/>
+      <c r="BO3" s="74"/>
+      <c r="BP3" s="74"/>
+      <c r="BQ3" s="74"/>
+      <c r="BR3" s="74"/>
+      <c r="BS3" s="74"/>
+      <c r="BT3" s="74"/>
+      <c r="BU3" s="74"/>
+      <c r="BV3" s="74"/>
+      <c r="BW3" s="74"/>
+      <c r="BX3" s="74"/>
+      <c r="BY3" s="74"/>
+      <c r="BZ3" s="74"/>
+      <c r="CA3" s="74"/>
+      <c r="CB3" s="74"/>
+      <c r="CC3" s="74"/>
+      <c r="CD3" s="74"/>
+      <c r="CE3" s="74"/>
+      <c r="CF3" s="74"/>
+      <c r="CG3" s="74"/>
+      <c r="CH3" s="74"/>
+      <c r="CI3" s="74"/>
+      <c r="CJ3" s="74"/>
+      <c r="CK3" s="74"/>
+      <c r="CL3" s="74"/>
+      <c r="CM3" s="74"/>
+      <c r="CN3" s="74"/>
+      <c r="CO3" s="74"/>
+      <c r="CP3" s="74"/>
+      <c r="CQ3" s="74"/>
+      <c r="CR3" s="74"/>
+      <c r="CS3" s="74"/>
+      <c r="CT3" s="74"/>
+      <c r="CU3" s="74"/>
+      <c r="CV3" s="74"/>
+      <c r="CW3" s="74"/>
+      <c r="CX3" s="74"/>
+      <c r="CY3" s="74"/>
+      <c r="CZ3" s="74"/>
+      <c r="DA3" s="74"/>
+      <c r="DB3" s="74"/>
+      <c r="DC3" s="75"/>
     </row>
     <row r="4" spans="2:107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="75" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="76"/>
-      <c r="AH4" s="76"/>
-      <c r="AI4" s="76"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
-      <c r="AN4" s="76"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="76"/>
-      <c r="AT4" s="76"/>
-      <c r="AU4" s="76"/>
-      <c r="AV4" s="76"/>
-      <c r="AW4" s="76"/>
-      <c r="AX4" s="76"/>
-      <c r="AY4" s="76"/>
-      <c r="AZ4" s="76"/>
-      <c r="BA4" s="76"/>
-      <c r="BB4" s="76"/>
-      <c r="BC4" s="76"/>
-      <c r="BD4" s="76"/>
-      <c r="BE4" s="76"/>
-      <c r="BF4" s="76"/>
-      <c r="BG4" s="76"/>
-      <c r="BH4" s="76"/>
-      <c r="BI4" s="76"/>
-      <c r="BJ4" s="76"/>
-      <c r="BK4" s="76"/>
-      <c r="BL4" s="76"/>
-      <c r="BM4" s="76"/>
-      <c r="BN4" s="76"/>
-      <c r="BO4" s="76"/>
-      <c r="BP4" s="76"/>
-      <c r="BQ4" s="76"/>
-      <c r="BR4" s="76"/>
-      <c r="BS4" s="76"/>
-      <c r="BT4" s="76"/>
-      <c r="BU4" s="76"/>
-      <c r="BV4" s="76"/>
-      <c r="BW4" s="76"/>
-      <c r="BX4" s="76"/>
-      <c r="BY4" s="76"/>
-      <c r="BZ4" s="76"/>
-      <c r="CA4" s="76"/>
-      <c r="CB4" s="76"/>
-      <c r="CC4" s="76"/>
-      <c r="CD4" s="76"/>
-      <c r="CE4" s="76"/>
-      <c r="CF4" s="76"/>
-      <c r="CG4" s="76"/>
-      <c r="CH4" s="76"/>
-      <c r="CI4" s="76"/>
-      <c r="CJ4" s="76"/>
-      <c r="CK4" s="76"/>
-      <c r="CL4" s="76"/>
-      <c r="CM4" s="76"/>
-      <c r="CN4" s="76"/>
-      <c r="CO4" s="76"/>
-      <c r="CP4" s="76"/>
-      <c r="CQ4" s="76"/>
-      <c r="CR4" s="76"/>
-      <c r="CS4" s="76"/>
-      <c r="CT4" s="76"/>
-      <c r="CU4" s="76"/>
-      <c r="CV4" s="76"/>
-      <c r="CW4" s="76"/>
-      <c r="CX4" s="76"/>
-      <c r="CY4" s="76"/>
-      <c r="CZ4" s="76"/>
-      <c r="DA4" s="76"/>
-      <c r="DB4" s="76"/>
-      <c r="DC4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="77"/>
+      <c r="AB4" s="77"/>
+      <c r="AC4" s="77"/>
+      <c r="AD4" s="77"/>
+      <c r="AE4" s="77"/>
+      <c r="AF4" s="77"/>
+      <c r="AG4" s="77"/>
+      <c r="AH4" s="77"/>
+      <c r="AI4" s="77"/>
+      <c r="AJ4" s="77"/>
+      <c r="AK4" s="77"/>
+      <c r="AL4" s="77"/>
+      <c r="AM4" s="77"/>
+      <c r="AN4" s="77"/>
+      <c r="AO4" s="77"/>
+      <c r="AP4" s="77"/>
+      <c r="AQ4" s="77"/>
+      <c r="AR4" s="77"/>
+      <c r="AS4" s="77"/>
+      <c r="AT4" s="77"/>
+      <c r="AU4" s="77"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="77"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="77"/>
+      <c r="BD4" s="77"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="77"/>
+      <c r="BG4" s="77"/>
+      <c r="BH4" s="77"/>
+      <c r="BI4" s="77"/>
+      <c r="BJ4" s="77"/>
+      <c r="BK4" s="77"/>
+      <c r="BL4" s="77"/>
+      <c r="BM4" s="77"/>
+      <c r="BN4" s="77"/>
+      <c r="BO4" s="77"/>
+      <c r="BP4" s="77"/>
+      <c r="BQ4" s="77"/>
+      <c r="BR4" s="77"/>
+      <c r="BS4" s="77"/>
+      <c r="BT4" s="77"/>
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="77"/>
+      <c r="BW4" s="77"/>
+      <c r="BX4" s="77"/>
+      <c r="BY4" s="77"/>
+      <c r="BZ4" s="77"/>
+      <c r="CA4" s="77"/>
+      <c r="CB4" s="77"/>
+      <c r="CC4" s="77"/>
+      <c r="CD4" s="77"/>
+      <c r="CE4" s="77"/>
+      <c r="CF4" s="77"/>
+      <c r="CG4" s="77"/>
+      <c r="CH4" s="77"/>
+      <c r="CI4" s="77"/>
+      <c r="CJ4" s="77"/>
+      <c r="CK4" s="77"/>
+      <c r="CL4" s="77"/>
+      <c r="CM4" s="77"/>
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="77"/>
+      <c r="CZ4" s="77"/>
+      <c r="DA4" s="77"/>
+      <c r="DB4" s="77"/>
+      <c r="DC4" s="78"/>
     </row>
     <row r="5" spans="2:107" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="44" t="s">

</xml_diff>